<commit_message>
Filtro no topo do app.
</commit_message>
<xml_diff>
--- a/PlanilhaDespezas.xlsx
+++ b/PlanilhaDespezas.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,68 +460,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R$ 400</t>
+          <t>R$ 900</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Trabalho</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Ganho</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>R$ 17000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cavalo vendido</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ganho</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>R$ 156.78</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Gasto</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>R$ 461.23</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pix tio paulo</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Gasto</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Funções de edição e exclusão adicionadas.
</commit_message>
<xml_diff>
--- a/PlanilhaDespezas.xlsx
+++ b/PlanilhaDespezas.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,17 +460,68 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R$ 900</t>
+          <t>R$ 2000.00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>Trabalho</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Ganho</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>R$ 1500</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Trabalho 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ganho</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>R$ 560.66</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>R$ 145.60</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Carro</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gasto</t>
         </is>
       </c>
     </row>

</xml_diff>